<commit_message>
added 1 point in exce Docemnt in future power
</commit_message>
<xml_diff>
--- a/Future Power/Document/Future Power costing.xlsx
+++ b/Future Power/Document/Future Power costing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MYDATA\Frelancing TDL\Documents\Future Power\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MYDATA\Frelancing TDL\TDL\Future Power\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880DC3FA-E478-43C2-9465-A67D86D6EB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4341EA-264C-4FB7-88CD-62D21D8856CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Customization</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>note: 1 Delivery Note or Receipt Note will be Controlled in sales and purchase</t>
+  </si>
+  <si>
+    <t>Stock Journal Import For Make Stock Item Closing balance zero</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
@@ -375,11 +381,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -390,7 +394,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -409,10 +415,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>3000</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>